<commit_message>
second workable app version
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Скважины</t>
+          <t>Скважина</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -450,7 +450,7 @@
         <v>1591</v>
       </c>
       <c r="B2" t="n">
-        <v>1.31</v>
+        <v>77.879</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         <v>1620</v>
       </c>
       <c r="B4" t="n">
-        <v>1.3</v>
+        <v>59.471</v>
       </c>
     </row>
     <row r="5">
@@ -470,7 +470,7 @@
         <v>1630</v>
       </c>
       <c r="B5" t="n">
-        <v>1.31</v>
+        <v>158.589</v>
       </c>
     </row>
     <row r="6">
@@ -482,7 +482,7 @@
         <v>1631</v>
       </c>
       <c r="B7" t="n">
-        <v>1.31</v>
+        <v>145.846</v>
       </c>
     </row>
     <row r="8">
@@ -494,7 +494,7 @@
         <v>1640</v>
       </c>
       <c r="B9" t="n">
-        <v>1.31</v>
+        <v>45.311</v>
       </c>
     </row>
     <row r="10">
@@ -502,7 +502,7 @@
         <v>1641</v>
       </c>
       <c r="B10" t="n">
-        <v>1.31</v>
+        <v>49.559</v>
       </c>
     </row>
     <row r="11">
@@ -510,7 +510,7 @@
         <v>1642</v>
       </c>
       <c r="B11" t="n">
-        <v>1.31</v>
+        <v>49.559</v>
       </c>
     </row>
     <row r="12">
@@ -518,7 +518,7 @@
         <v>1650</v>
       </c>
       <c r="B12" t="n">
-        <v>1.31</v>
+        <v>62.303</v>
       </c>
     </row>
     <row r="13">
@@ -526,7 +526,7 @@
         <v>1651</v>
       </c>
       <c r="B13" t="n">
-        <v>1.31</v>
+        <v>100.534</v>
       </c>
     </row>
     <row r="14">
@@ -534,7 +534,7 @@
         <v>1660</v>
       </c>
       <c r="B14" t="n">
-        <v>1.31</v>
+        <v>56.639</v>
       </c>
     </row>
     <row r="15">
@@ -542,7 +542,7 @@
         <v>1661</v>
       </c>
       <c r="B15" t="n">
-        <v>1.31</v>
+        <v>56.639</v>
       </c>
     </row>
     <row r="16">
@@ -550,7 +550,7 @@
         <v>1662</v>
       </c>
       <c r="B16" t="n">
-        <v>1.31</v>
+        <v>84.958</v>
       </c>
     </row>
     <row r="17">
@@ -558,7 +558,7 @@
         <v>1670</v>
       </c>
       <c r="B17" t="n">
-        <v>1.31</v>
+        <v>49.559</v>
       </c>
     </row>
     <row r="18">
@@ -566,7 +566,7 @@
         <v>1671</v>
       </c>
       <c r="B18" t="n">
-        <v>1.31</v>
+        <v>131.686</v>
       </c>
     </row>
     <row r="19">
@@ -574,7 +574,7 @@
         <v>1680</v>
       </c>
       <c r="B19" t="n">
-        <v>1.31</v>
+        <v>222.308</v>
       </c>
     </row>
     <row r="20">
@@ -582,7 +582,7 @@
         <v>1681</v>
       </c>
       <c r="B20" t="n">
-        <v>1.31</v>
+        <v>133.102</v>
       </c>
     </row>
     <row r="21">
@@ -594,7 +594,7 @@
         <v>1682</v>
       </c>
       <c r="B22" t="n">
-        <v>1.31</v>
+        <v>70.79900000000001</v>
       </c>
     </row>
     <row r="23">
@@ -606,7 +606,7 @@
         <v>1690</v>
       </c>
       <c r="B24" t="n">
-        <v>1.32</v>
+        <v>65.13500000000001</v>
       </c>
     </row>
     <row r="25">
@@ -614,7 +614,7 @@
         <v>1691</v>
       </c>
       <c r="B25" t="n">
-        <v>1.32</v>
+        <v>46.727</v>
       </c>
     </row>
     <row r="26">
@@ -622,7 +622,7 @@
         <v>1700</v>
       </c>
       <c r="B26" t="n">
-        <v>1.32</v>
+        <v>41.063</v>
       </c>
     </row>
     <row r="27">
@@ -630,7 +630,7 @@
         <v>1701</v>
       </c>
       <c r="B27" t="n">
-        <v>1.32</v>
+        <v>123.19</v>
       </c>
     </row>
     <row r="28">
@@ -638,7 +638,7 @@
         <v>1702</v>
       </c>
       <c r="B28" t="n">
-        <v>1.32</v>
+        <v>169.917</v>
       </c>
     </row>
     <row r="29">
@@ -646,7 +646,7 @@
         <v>1710</v>
       </c>
       <c r="B29" t="n">
-        <v>1.31</v>
+        <v>150.093</v>
       </c>
     </row>
     <row r="30">
@@ -654,7 +654,7 @@
         <v>1711</v>
       </c>
       <c r="B30" t="n">
-        <v>1.31</v>
+        <v>77.879</v>
       </c>
     </row>
     <row r="31">
@@ -662,7 +662,7 @@
         <v>1720</v>
       </c>
       <c r="B31" t="n">
-        <v>1.32</v>
+        <v>79.295</v>
       </c>
     </row>
     <row r="32">
@@ -670,7 +670,7 @@
         <v>1721</v>
       </c>
       <c r="B32" t="n">
-        <v>1.32</v>
+        <v>155.757</v>
       </c>
     </row>
     <row r="33">
@@ -686,7 +686,7 @@
         <v>1730</v>
       </c>
       <c r="B35" t="n">
-        <v>1.31</v>
+        <v>178.413</v>
       </c>
     </row>
     <row r="36">
@@ -694,7 +694,7 @@
         <v>1731</v>
       </c>
       <c r="B36" t="n">
-        <v>1.31</v>
+        <v>35.399</v>
       </c>
     </row>
     <row r="37">
@@ -702,7 +702,7 @@
         <v>1740</v>
       </c>
       <c r="B37" t="n">
-        <v>1.32</v>
+        <v>66.551</v>
       </c>
     </row>
     <row r="38">
@@ -714,7 +714,7 @@
         <v>1741</v>
       </c>
       <c r="B39" t="n">
-        <v>1.32</v>
+        <v>150.093</v>
       </c>
     </row>
     <row r="40">
@@ -722,7 +722,7 @@
         <v>1750</v>
       </c>
       <c r="B40" t="n">
-        <v>1.31</v>
+        <v>175.581</v>
       </c>
     </row>
     <row r="41">
@@ -730,7 +730,7 @@
         <v>1751</v>
       </c>
       <c r="B41" t="n">
-        <v>1.31</v>
+        <v>94.87</v>
       </c>
     </row>
     <row r="42">
@@ -742,7 +742,7 @@
         <v>1752</v>
       </c>
       <c r="B43" t="n">
-        <v>1.31</v>
+        <v>101.95</v>
       </c>
     </row>
     <row r="44">
@@ -750,7 +750,7 @@
         <v>1770</v>
       </c>
       <c r="B44" t="n">
-        <v>1.32</v>
+        <v>172.749</v>
       </c>
     </row>
     <row r="45">
@@ -762,7 +762,7 @@
         <v>1771</v>
       </c>
       <c r="B46" t="n">
-        <v>1.32</v>
+        <v>185.493</v>
       </c>
     </row>
     <row r="47">
@@ -770,7 +770,7 @@
         <v>1780</v>
       </c>
       <c r="B47" t="n">
-        <v>1.32</v>
+        <v>147.262</v>
       </c>
     </row>
     <row r="48">
@@ -778,7 +778,7 @@
         <v>1781</v>
       </c>
       <c r="B48" t="n">
-        <v>1.32</v>
+        <v>143.014</v>
       </c>
     </row>
     <row r="49">
@@ -786,7 +786,7 @@
         <v>1782</v>
       </c>
       <c r="B49" t="n">
-        <v>1.32</v>
+        <v>113.278</v>
       </c>
     </row>
     <row r="50">
@@ -794,7 +794,7 @@
         <v>1790</v>
       </c>
       <c r="B50" t="n">
-        <v>1.31</v>
+        <v>97.702</v>
       </c>
     </row>
     <row r="51">
@@ -802,7 +802,7 @@
         <v>1791</v>
       </c>
       <c r="B51" t="n">
-        <v>1.31</v>
+        <v>134.518</v>
       </c>
     </row>
     <row r="52">
@@ -810,7 +810,7 @@
         <v>1792</v>
       </c>
       <c r="B52" t="n">
-        <v>1.31</v>
+        <v>82.127</v>
       </c>
     </row>
     <row r="53">
@@ -818,7 +818,7 @@
         <v>1800</v>
       </c>
       <c r="B53" t="n">
-        <v>1.32</v>
+        <v>162.837</v>
       </c>
     </row>
     <row r="54">
@@ -826,7 +826,7 @@
         <v>1801</v>
       </c>
       <c r="B54" t="n">
-        <v>1.32</v>
+        <v>209.564</v>
       </c>
     </row>
     <row r="55">
@@ -834,7 +834,7 @@
         <v>1802</v>
       </c>
       <c r="B55" t="n">
-        <v>1.32</v>
+        <v>191.157</v>
       </c>
     </row>
     <row r="56">
@@ -842,7 +842,7 @@
         <v>1810</v>
       </c>
       <c r="B56" t="n">
-        <v>1.31</v>
+        <v>277.531</v>
       </c>
     </row>
     <row r="57">
@@ -850,7 +850,7 @@
         <v>1811</v>
       </c>
       <c r="B57" t="n">
-        <v>1.31</v>
+        <v>107.614</v>
       </c>
     </row>
     <row r="58">
@@ -858,7 +858,7 @@
         <v>1812</v>
       </c>
       <c r="B58" t="n">
-        <v>1.31</v>
+        <v>254.876</v>
       </c>
     </row>
     <row r="59">
@@ -866,7 +866,7 @@
         <v>1820</v>
       </c>
       <c r="B59" t="n">
-        <v>1.31</v>
+        <v>199.653</v>
       </c>
     </row>
     <row r="60">
@@ -874,7 +874,7 @@
         <v>1821</v>
       </c>
       <c r="B60" t="n">
-        <v>1.31</v>
+        <v>176.997</v>
       </c>
     </row>
     <row r="61">
@@ -882,7 +882,7 @@
         <v>1822</v>
       </c>
       <c r="B61" t="n">
-        <v>1.31</v>
+        <v>67.967</v>
       </c>
     </row>
     <row r="62">
@@ -890,7 +890,7 @@
         <v>1830</v>
       </c>
       <c r="B62" t="n">
-        <v>1.32</v>
+        <v>150.093</v>
       </c>
     </row>
     <row r="63">
@@ -898,7 +898,7 @@
         <v>1831</v>
       </c>
       <c r="B63" t="n">
-        <v>1.32</v>
+        <v>145.846</v>
       </c>
     </row>
     <row r="64">
@@ -906,7 +906,7 @@
         <v>1832</v>
       </c>
       <c r="B64" t="n">
-        <v>1.32</v>
+        <v>137.35</v>
       </c>
     </row>
     <row r="65">
@@ -914,7 +914,7 @@
         <v>1840</v>
       </c>
       <c r="B65" t="n">
-        <v>1.33</v>
+        <v>281.779</v>
       </c>
     </row>
     <row r="66">
@@ -922,7 +922,7 @@
         <v>1841</v>
       </c>
       <c r="B66" t="n">
-        <v>1.33</v>
+        <v>281.779</v>
       </c>
     </row>
     <row r="67">
@@ -930,7 +930,7 @@
         <v>1842</v>
       </c>
       <c r="B67" t="n">
-        <v>1.33</v>
+        <v>222.308</v>
       </c>
     </row>
     <row r="68">
@@ -938,7 +938,7 @@
         <v>1850</v>
       </c>
       <c r="B68" t="n">
-        <v>1.31</v>
+        <v>181.245</v>
       </c>
     </row>
     <row r="69">
@@ -946,7 +946,7 @@
         <v>1851</v>
       </c>
       <c r="B69" t="n">
-        <v>1.31</v>
+        <v>107.614</v>
       </c>
     </row>
     <row r="70">
@@ -954,7 +954,7 @@
         <v>1860</v>
       </c>
       <c r="B70" t="n">
-        <v>1.32</v>
+        <v>168.501</v>
       </c>
     </row>
     <row r="71">
@@ -962,7 +962,7 @@
         <v>1861</v>
       </c>
       <c r="B71" t="n">
-        <v>1.32</v>
+        <v>178.413</v>
       </c>
     </row>
     <row r="72">
@@ -970,7 +970,7 @@
         <v>1863</v>
       </c>
       <c r="B72" t="n">
-        <v>1.32</v>
+        <v>300.187</v>
       </c>
     </row>
     <row r="73">
@@ -978,7 +978,7 @@
         <v>1870</v>
       </c>
       <c r="B73" t="n">
-        <v>1.31</v>
+        <v>184.077</v>
       </c>
     </row>
     <row r="74">
@@ -986,7 +986,7 @@
         <v>1871</v>
       </c>
       <c r="B74" t="n">
-        <v>1.31</v>
+        <v>117.526</v>
       </c>
     </row>
     <row r="75">
@@ -994,7 +994,7 @@
         <v>1872</v>
       </c>
       <c r="B75" t="n">
-        <v>1.31</v>
+        <v>152.925</v>
       </c>
     </row>
     <row r="76">
@@ -1002,7 +1002,7 @@
         <v>1880</v>
       </c>
       <c r="B76" t="n">
-        <v>1.33</v>
+        <v>218.06</v>
       </c>
     </row>
     <row r="77">
@@ -1010,7 +1010,7 @@
         <v>1881</v>
       </c>
       <c r="B77" t="n">
-        <v>1.33</v>
+        <v>151.509</v>
       </c>
     </row>
     <row r="78">
@@ -1018,7 +1018,7 @@
         <v>1882</v>
       </c>
       <c r="B78" t="n">
-        <v>1.33</v>
+        <v>154.341</v>
       </c>
     </row>
     <row r="79">
@@ -1030,7 +1030,7 @@
         <v>1890</v>
       </c>
       <c r="B80" t="n">
-        <v>1.2</v>
+        <v>271.867</v>
       </c>
     </row>
     <row r="81">
@@ -1038,7 +1038,7 @@
         <v>1891</v>
       </c>
       <c r="B81" t="n">
-        <v>1.2</v>
+        <v>94.87</v>
       </c>
     </row>
     <row r="82">
@@ -1046,7 +1046,7 @@
         <v>1900</v>
       </c>
       <c r="B82" t="n">
-        <v>1.31</v>
+        <v>249.212</v>
       </c>
     </row>
     <row r="83">
@@ -1058,15 +1058,15 @@
         <v>1901</v>
       </c>
       <c r="B84" t="n">
-        <v>1.31</v>
+        <v>312.931</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>1.4</v>
+        <v>1254.7</v>
       </c>
       <c r="B85" t="n">
-        <v>1.31</v>
+        <v>77.879</v>
       </c>
     </row>
     <row r="86">
@@ -1075,18 +1075,18 @@
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>0</v>
+        <v>1166.85</v>
       </c>
       <c r="B87" t="n">
-        <v>1.3</v>
+        <v>59.471</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>0</v>
+        <v>1193.92</v>
       </c>
       <c r="B88" t="n">
-        <v>1.31</v>
+        <v>158.589</v>
       </c>
     </row>
     <row r="89">
@@ -1095,10 +1095,10 @@
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>0</v>
+        <v>1218.9</v>
       </c>
       <c r="B90" t="n">
-        <v>1.31</v>
+        <v>145.846</v>
       </c>
     </row>
     <row r="91">
@@ -1107,98 +1107,98 @@
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>1.4</v>
+        <v>1160</v>
       </c>
       <c r="B92" t="n">
-        <v>1.31</v>
+        <v>45.311</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>1.7</v>
+        <v>1174.4</v>
       </c>
       <c r="B93" t="n">
-        <v>1.31</v>
+        <v>49.559</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>0</v>
+        <v>1185.4</v>
       </c>
       <c r="B94" t="n">
-        <v>1.31</v>
+        <v>49.559</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>0</v>
+        <v>1169.5</v>
       </c>
       <c r="B95" t="n">
-        <v>1.31</v>
+        <v>62.303</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>0</v>
+        <v>1185.77</v>
       </c>
       <c r="B96" t="n">
-        <v>1.31</v>
+        <v>100.534</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>0</v>
+        <v>1161.72</v>
       </c>
       <c r="B97" t="n">
-        <v>1.31</v>
+        <v>56.639</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>0</v>
+        <v>1159</v>
       </c>
       <c r="B98" t="n">
-        <v>1.31</v>
+        <v>56.639</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>0</v>
+        <v>1175.5</v>
       </c>
       <c r="B99" t="n">
-        <v>1.31</v>
+        <v>84.958</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>0</v>
+        <v>1173.5</v>
       </c>
       <c r="B100" t="n">
-        <v>1.31</v>
+        <v>49.559</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>0</v>
+        <v>1213.2</v>
       </c>
       <c r="B101" t="n">
-        <v>1.31</v>
+        <v>131.686</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>0</v>
+        <v>1132.3</v>
       </c>
       <c r="B102" t="n">
-        <v>1.31</v>
+        <v>222.308</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>1.4</v>
+        <v>1218.2</v>
       </c>
       <c r="B103" t="n">
-        <v>1.31</v>
+        <v>133.102</v>
       </c>
     </row>
     <row r="104">
@@ -1207,86 +1207,88 @@
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>0</v>
+        <v>1018.36</v>
       </c>
       <c r="B105" t="n">
-        <v>1.31</v>
+        <v>70.79900000000001</v>
       </c>
     </row>
     <row r="106">
-      <c r="A106" t="inlineStr"/>
+      <c r="A106" t="n">
+        <v>1198.9</v>
+      </c>
       <c r="B106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>0</v>
+        <v>1159.77</v>
       </c>
       <c r="B107" t="n">
-        <v>1.32</v>
+        <v>65.13500000000001</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>0</v>
+        <v>1191.2</v>
       </c>
       <c r="B108" t="n">
-        <v>1.32</v>
+        <v>46.727</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>0</v>
+        <v>1180.3</v>
       </c>
       <c r="B109" t="n">
-        <v>1.32</v>
+        <v>41.063</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>0</v>
+        <v>1214.4</v>
       </c>
       <c r="B110" t="n">
-        <v>1.32</v>
+        <v>123.19</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>0</v>
+        <v>1135.6</v>
       </c>
       <c r="B111" t="n">
-        <v>1.32</v>
+        <v>169.917</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>0</v>
+        <v>1152.3</v>
       </c>
       <c r="B112" t="n">
-        <v>1.31</v>
+        <v>150.093</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>0</v>
+        <v>1211.95</v>
       </c>
       <c r="B113" t="n">
-        <v>1.31</v>
+        <v>77.879</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>0</v>
+        <v>1201.8</v>
       </c>
       <c r="B114" t="n">
-        <v>1.32</v>
+        <v>79.295</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>0</v>
+        <v>1163.1</v>
       </c>
       <c r="B115" t="n">
-        <v>1.32</v>
+        <v>155.757</v>
       </c>
     </row>
     <row r="116">
@@ -1299,26 +1301,26 @@
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>0</v>
+        <v>1172.9</v>
       </c>
       <c r="B118" t="n">
-        <v>1.31</v>
+        <v>178.413</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>0</v>
+        <v>1175.4</v>
       </c>
       <c r="B119" t="n">
-        <v>1.31</v>
+        <v>35.399</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>0</v>
+        <v>1175.7</v>
       </c>
       <c r="B120" t="n">
-        <v>1.32</v>
+        <v>66.551</v>
       </c>
     </row>
     <row r="121">
@@ -1327,26 +1329,26 @@
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>0</v>
+        <v>1183.2</v>
       </c>
       <c r="B122" t="n">
-        <v>1.32</v>
+        <v>150.093</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>1.2</v>
+        <v>1184.8</v>
       </c>
       <c r="B123" t="n">
-        <v>1.31</v>
+        <v>175.581</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>0</v>
+        <v>1173.4</v>
       </c>
       <c r="B124" t="n">
-        <v>1.31</v>
+        <v>94.87</v>
       </c>
     </row>
     <row r="125">
@@ -1355,286 +1357,288 @@
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>0.4</v>
+        <v>1184.57</v>
       </c>
       <c r="B126" t="n">
-        <v>1.31</v>
+        <v>101.95</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>0</v>
+        <v>941.5</v>
       </c>
       <c r="B127" t="n">
-        <v>1.32</v>
+        <v>172.749</v>
       </c>
     </row>
     <row r="128">
-      <c r="A128" t="inlineStr"/>
+      <c r="A128" t="n">
+        <v>1155.9</v>
+      </c>
       <c r="B128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>0</v>
+        <v>1159.7</v>
       </c>
       <c r="B129" t="n">
-        <v>1.32</v>
+        <v>185.493</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>0</v>
+        <v>1184.7</v>
       </c>
       <c r="B130" t="n">
-        <v>1.32</v>
+        <v>147.262</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>0</v>
+        <v>1188.9</v>
       </c>
       <c r="B131" t="n">
-        <v>1.32</v>
+        <v>143.014</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>0</v>
+        <v>1181.2</v>
       </c>
       <c r="B132" t="n">
-        <v>1.32</v>
+        <v>113.278</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>0</v>
+        <v>1143.8</v>
       </c>
       <c r="B133" t="n">
-        <v>1.31</v>
+        <v>97.702</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>0</v>
+        <v>1224.3</v>
       </c>
       <c r="B134" t="n">
-        <v>1.31</v>
+        <v>134.518</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>0</v>
+        <v>1189.9</v>
       </c>
       <c r="B135" t="n">
-        <v>1.31</v>
+        <v>82.127</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>0</v>
+        <v>1203.4</v>
       </c>
       <c r="B136" t="n">
-        <v>1.32</v>
+        <v>162.837</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>0</v>
+        <v>1153</v>
       </c>
       <c r="B137" t="n">
-        <v>1.32</v>
+        <v>209.564</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>0</v>
+        <v>1178.8</v>
       </c>
       <c r="B138" t="n">
-        <v>1.32</v>
+        <v>191.157</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>0</v>
+        <v>1183.8</v>
       </c>
       <c r="B139" t="n">
-        <v>1.31</v>
+        <v>277.531</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>0</v>
+        <v>1214.7</v>
       </c>
       <c r="B140" t="n">
-        <v>1.31</v>
+        <v>107.614</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>0</v>
+        <v>1154.2</v>
       </c>
       <c r="B141" t="n">
-        <v>1.31</v>
+        <v>254.876</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>0</v>
+        <v>1201.8</v>
       </c>
       <c r="B142" t="n">
-        <v>1.31</v>
+        <v>199.653</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>0</v>
+        <v>1164.7</v>
       </c>
       <c r="B143" t="n">
-        <v>1.31</v>
+        <v>176.997</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>0</v>
+        <v>1202.19</v>
       </c>
       <c r="B144" t="n">
-        <v>1.31</v>
+        <v>67.967</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>0</v>
+        <v>1181.3</v>
       </c>
       <c r="B145" t="n">
-        <v>1.32</v>
+        <v>150.093</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>0</v>
+        <v>1166.2</v>
       </c>
       <c r="B146" t="n">
-        <v>1.32</v>
+        <v>145.846</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>1.6</v>
+        <v>1175.27</v>
       </c>
       <c r="B147" t="n">
-        <v>1.32</v>
+        <v>137.35</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>0</v>
+        <v>1210.3</v>
       </c>
       <c r="B148" t="n">
-        <v>1.33</v>
+        <v>281.779</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>0</v>
+        <v>1174.1</v>
       </c>
       <c r="B149" t="n">
-        <v>1.33</v>
+        <v>281.779</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>0</v>
+        <v>1222.7</v>
       </c>
       <c r="B150" t="n">
-        <v>1.33</v>
+        <v>222.308</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>0</v>
+        <v>1160.4</v>
       </c>
       <c r="B151" t="n">
-        <v>1.31</v>
+        <v>181.245</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>0</v>
+        <v>1146.8</v>
       </c>
       <c r="B152" t="n">
-        <v>1.31</v>
+        <v>107.614</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>0</v>
+        <v>1189.9</v>
       </c>
       <c r="B153" t="n">
-        <v>1.32</v>
+        <v>168.501</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>0</v>
+        <v>1209.5</v>
       </c>
       <c r="B154" t="n">
-        <v>1.32</v>
+        <v>178.413</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>0</v>
+        <v>1184.5</v>
       </c>
       <c r="B155" t="n">
-        <v>1.32</v>
+        <v>300.187</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>0</v>
+        <v>1182.5</v>
       </c>
       <c r="B156" t="n">
-        <v>1.31</v>
+        <v>184.077</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="n">
-        <v>1.2</v>
+        <v>1189</v>
       </c>
       <c r="B157" t="n">
-        <v>1.31</v>
+        <v>117.526</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="n">
-        <v>0</v>
+        <v>1216.5</v>
       </c>
       <c r="B158" t="n">
-        <v>1.31</v>
+        <v>152.925</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>0</v>
+        <v>1175</v>
       </c>
       <c r="B159" t="n">
-        <v>1.33</v>
+        <v>218.06</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>1.3</v>
+        <v>1141.9</v>
       </c>
       <c r="B160" t="n">
-        <v>1.33</v>
+        <v>151.509</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="n">
-        <v>0</v>
+        <v>1228</v>
       </c>
       <c r="B161" t="n">
-        <v>1.33</v>
+        <v>154.341</v>
       </c>
     </row>
     <row r="162">
@@ -1643,26 +1647,26 @@
     </row>
     <row r="163">
       <c r="A163" t="n">
-        <v>0</v>
+        <v>1154.6</v>
       </c>
       <c r="B163" t="n">
-        <v>1.2</v>
+        <v>271.867</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="n">
-        <v>0</v>
+        <v>1172.04</v>
       </c>
       <c r="B164" t="n">
-        <v>1.2</v>
+        <v>94.87</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="n">
-        <v>0</v>
+        <v>1203.9</v>
       </c>
       <c r="B165" t="n">
-        <v>1.31</v>
+        <v>249.212</v>
       </c>
     </row>
     <row r="166">
@@ -1671,18 +1675,18 @@
     </row>
     <row r="167">
       <c r="A167" t="n">
-        <v>1.7</v>
+        <v>1160.7</v>
       </c>
       <c r="B167" t="n">
-        <v>1.31</v>
+        <v>312.931</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="n">
-        <v>1.31</v>
+        <v>77.879</v>
       </c>
       <c r="B168" t="n">
-        <v>1.31</v>
+        <v>77.879</v>
       </c>
     </row>
     <row r="169">
@@ -1691,18 +1695,18 @@
     </row>
     <row r="170">
       <c r="A170" t="n">
-        <v>1.3</v>
+        <v>59.471</v>
       </c>
       <c r="B170" t="n">
-        <v>1.3</v>
+        <v>59.471</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>1.31</v>
+        <v>158.589</v>
       </c>
       <c r="B171" t="n">
-        <v>1.31</v>
+        <v>158.589</v>
       </c>
     </row>
     <row r="172">
@@ -1711,10 +1715,10 @@
     </row>
     <row r="173">
       <c r="A173" t="n">
-        <v>1.31</v>
+        <v>145.846</v>
       </c>
       <c r="B173" t="n">
-        <v>1.31</v>
+        <v>145.846</v>
       </c>
     </row>
     <row r="174">
@@ -1723,98 +1727,98 @@
     </row>
     <row r="175">
       <c r="A175" t="n">
-        <v>1.31</v>
+        <v>45.311</v>
       </c>
       <c r="B175" t="n">
-        <v>1.31</v>
+        <v>45.311</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="n">
-        <v>1.31</v>
+        <v>49.559</v>
       </c>
       <c r="B176" t="n">
-        <v>1.31</v>
+        <v>49.559</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="n">
-        <v>1.31</v>
+        <v>49.559</v>
       </c>
       <c r="B177" t="n">
-        <v>1.31</v>
+        <v>49.559</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="n">
-        <v>1.31</v>
+        <v>62.303</v>
       </c>
       <c r="B178" t="n">
-        <v>1.31</v>
+        <v>62.303</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="n">
-        <v>1.31</v>
+        <v>100.534</v>
       </c>
       <c r="B179" t="n">
-        <v>1.31</v>
+        <v>100.534</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="n">
-        <v>1.31</v>
+        <v>56.639</v>
       </c>
       <c r="B180" t="n">
-        <v>1.31</v>
+        <v>56.639</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="n">
-        <v>1.31</v>
+        <v>56.639</v>
       </c>
       <c r="B181" t="n">
-        <v>1.31</v>
+        <v>56.639</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="n">
-        <v>1.31</v>
+        <v>84.958</v>
       </c>
       <c r="B182" t="n">
-        <v>1.31</v>
+        <v>84.958</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="n">
-        <v>1.31</v>
+        <v>49.559</v>
       </c>
       <c r="B183" t="n">
-        <v>1.31</v>
+        <v>49.559</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="n">
-        <v>1.31</v>
+        <v>131.686</v>
       </c>
       <c r="B184" t="n">
-        <v>1.31</v>
+        <v>131.686</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="n">
-        <v>1.31</v>
+        <v>222.308</v>
       </c>
       <c r="B185" t="n">
-        <v>1.31</v>
+        <v>222.308</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="n">
-        <v>1.31</v>
+        <v>133.102</v>
       </c>
       <c r="B186" t="n">
-        <v>1.31</v>
+        <v>133.102</v>
       </c>
     </row>
     <row r="187">
@@ -1823,10 +1827,10 @@
     </row>
     <row r="188">
       <c r="A188" t="n">
-        <v>1.31</v>
+        <v>70.79900000000001</v>
       </c>
       <c r="B188" t="n">
-        <v>1.31</v>
+        <v>70.79900000000001</v>
       </c>
     </row>
     <row r="189">
@@ -1835,74 +1839,74 @@
     </row>
     <row r="190">
       <c r="A190" t="n">
-        <v>1.32</v>
+        <v>65.13500000000001</v>
       </c>
       <c r="B190" t="n">
-        <v>1.32</v>
+        <v>65.13500000000001</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="n">
-        <v>1.32</v>
+        <v>46.727</v>
       </c>
       <c r="B191" t="n">
-        <v>1.32</v>
+        <v>46.727</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="n">
-        <v>1.32</v>
+        <v>41.063</v>
       </c>
       <c r="B192" t="n">
-        <v>1.32</v>
+        <v>41.063</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="n">
-        <v>1.32</v>
+        <v>123.19</v>
       </c>
       <c r="B193" t="n">
-        <v>1.32</v>
+        <v>123.19</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="n">
-        <v>1.32</v>
+        <v>169.917</v>
       </c>
       <c r="B194" t="n">
-        <v>1.32</v>
+        <v>169.917</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="n">
-        <v>1.31</v>
+        <v>150.093</v>
       </c>
       <c r="B195" t="n">
-        <v>1.31</v>
+        <v>150.093</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="n">
-        <v>1.31</v>
+        <v>77.879</v>
       </c>
       <c r="B196" t="n">
-        <v>1.31</v>
+        <v>77.879</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="n">
-        <v>1.32</v>
+        <v>79.295</v>
       </c>
       <c r="B197" t="n">
-        <v>1.32</v>
+        <v>79.295</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="n">
-        <v>1.32</v>
+        <v>155.757</v>
       </c>
       <c r="B198" t="n">
-        <v>1.32</v>
+        <v>155.757</v>
       </c>
     </row>
     <row r="199">
@@ -1915,26 +1919,26 @@
     </row>
     <row r="201">
       <c r="A201" t="n">
-        <v>1.31</v>
+        <v>178.413</v>
       </c>
       <c r="B201" t="n">
-        <v>1.31</v>
+        <v>178.413</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="n">
-        <v>1.31</v>
+        <v>35.399</v>
       </c>
       <c r="B202" t="n">
-        <v>1.31</v>
+        <v>35.399</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="n">
-        <v>1.32</v>
+        <v>66.551</v>
       </c>
       <c r="B203" t="n">
-        <v>1.32</v>
+        <v>66.551</v>
       </c>
     </row>
     <row r="204">
@@ -1943,26 +1947,26 @@
     </row>
     <row r="205">
       <c r="A205" t="n">
-        <v>1.32</v>
+        <v>150.093</v>
       </c>
       <c r="B205" t="n">
-        <v>1.32</v>
+        <v>150.093</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="n">
-        <v>1.31</v>
+        <v>175.581</v>
       </c>
       <c r="B206" t="n">
-        <v>1.31</v>
+        <v>175.581</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="n">
-        <v>1.31</v>
+        <v>94.87</v>
       </c>
       <c r="B207" t="n">
-        <v>1.31</v>
+        <v>94.87</v>
       </c>
     </row>
     <row r="208">
@@ -1971,18 +1975,18 @@
     </row>
     <row r="209">
       <c r="A209" t="n">
-        <v>1.31</v>
+        <v>101.95</v>
       </c>
       <c r="B209" t="n">
-        <v>1.31</v>
+        <v>101.95</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="n">
-        <v>1.32</v>
+        <v>172.749</v>
       </c>
       <c r="B210" t="n">
-        <v>1.32</v>
+        <v>172.749</v>
       </c>
     </row>
     <row r="211">
@@ -1991,266 +1995,266 @@
     </row>
     <row r="212">
       <c r="A212" t="n">
-        <v>1.32</v>
+        <v>185.493</v>
       </c>
       <c r="B212" t="n">
-        <v>1.32</v>
+        <v>185.493</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="n">
-        <v>1.32</v>
+        <v>147.262</v>
       </c>
       <c r="B213" t="n">
-        <v>1.32</v>
+        <v>147.262</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="n">
-        <v>1.32</v>
+        <v>143.014</v>
       </c>
       <c r="B214" t="n">
-        <v>1.32</v>
+        <v>143.014</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="n">
-        <v>1.32</v>
+        <v>113.278</v>
       </c>
       <c r="B215" t="n">
-        <v>1.32</v>
+        <v>113.278</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="n">
-        <v>1.31</v>
+        <v>97.702</v>
       </c>
       <c r="B216" t="n">
-        <v>1.31</v>
+        <v>97.702</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="n">
-        <v>1.31</v>
+        <v>134.518</v>
       </c>
       <c r="B217" t="n">
-        <v>1.31</v>
+        <v>134.518</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="n">
-        <v>1.31</v>
+        <v>82.127</v>
       </c>
       <c r="B218" t="n">
-        <v>1.31</v>
+        <v>82.127</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="n">
-        <v>1.32</v>
+        <v>162.837</v>
       </c>
       <c r="B219" t="n">
-        <v>1.32</v>
+        <v>162.837</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="n">
-        <v>1.32</v>
+        <v>209.564</v>
       </c>
       <c r="B220" t="n">
-        <v>1.32</v>
+        <v>209.564</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="n">
-        <v>1.32</v>
+        <v>191.157</v>
       </c>
       <c r="B221" t="n">
-        <v>1.32</v>
+        <v>191.157</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="n">
-        <v>1.31</v>
+        <v>277.531</v>
       </c>
       <c r="B222" t="n">
-        <v>1.31</v>
+        <v>277.531</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="n">
-        <v>1.31</v>
+        <v>107.614</v>
       </c>
       <c r="B223" t="n">
-        <v>1.31</v>
+        <v>107.614</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="n">
-        <v>1.31</v>
+        <v>254.876</v>
       </c>
       <c r="B224" t="n">
-        <v>1.31</v>
+        <v>254.876</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="n">
-        <v>1.31</v>
+        <v>199.653</v>
       </c>
       <c r="B225" t="n">
-        <v>1.31</v>
+        <v>199.653</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="n">
-        <v>1.31</v>
+        <v>176.997</v>
       </c>
       <c r="B226" t="n">
-        <v>1.31</v>
+        <v>176.997</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="n">
-        <v>1.31</v>
+        <v>67.967</v>
       </c>
       <c r="B227" t="n">
-        <v>1.31</v>
+        <v>67.967</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="n">
-        <v>1.32</v>
+        <v>150.093</v>
       </c>
       <c r="B228" t="n">
-        <v>1.32</v>
+        <v>150.093</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="n">
-        <v>1.32</v>
+        <v>145.846</v>
       </c>
       <c r="B229" t="n">
-        <v>1.32</v>
+        <v>145.846</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="n">
-        <v>1.32</v>
+        <v>137.35</v>
       </c>
       <c r="B230" t="n">
-        <v>1.32</v>
+        <v>137.35</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="n">
-        <v>1.33</v>
+        <v>281.779</v>
       </c>
       <c r="B231" t="n">
-        <v>1.33</v>
+        <v>281.779</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="n">
-        <v>1.33</v>
+        <v>281.779</v>
       </c>
       <c r="B232" t="n">
-        <v>1.33</v>
+        <v>281.779</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="n">
-        <v>1.33</v>
+        <v>222.308</v>
       </c>
       <c r="B233" t="n">
-        <v>1.33</v>
+        <v>222.308</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="n">
-        <v>1.31</v>
+        <v>181.245</v>
       </c>
       <c r="B234" t="n">
-        <v>1.31</v>
+        <v>181.245</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="n">
-        <v>1.31</v>
+        <v>107.614</v>
       </c>
       <c r="B235" t="n">
-        <v>1.31</v>
+        <v>107.614</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="n">
-        <v>1.32</v>
+        <v>168.501</v>
       </c>
       <c r="B236" t="n">
-        <v>1.32</v>
+        <v>168.501</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="n">
-        <v>1.32</v>
+        <v>178.413</v>
       </c>
       <c r="B237" t="n">
-        <v>1.32</v>
+        <v>178.413</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="n">
-        <v>1.32</v>
+        <v>300.187</v>
       </c>
       <c r="B238" t="n">
-        <v>1.32</v>
+        <v>300.187</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="n">
-        <v>1.31</v>
+        <v>184.077</v>
       </c>
       <c r="B239" t="n">
-        <v>1.31</v>
+        <v>184.077</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="n">
-        <v>1.31</v>
+        <v>117.526</v>
       </c>
       <c r="B240" t="n">
-        <v>1.31</v>
+        <v>117.526</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="n">
-        <v>1.31</v>
+        <v>152.925</v>
       </c>
       <c r="B241" t="n">
-        <v>1.31</v>
+        <v>152.925</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="n">
-        <v>1.33</v>
+        <v>218.06</v>
       </c>
       <c r="B242" t="n">
-        <v>1.33</v>
+        <v>218.06</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="n">
-        <v>1.33</v>
+        <v>151.509</v>
       </c>
       <c r="B243" t="n">
-        <v>1.33</v>
+        <v>151.509</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="n">
-        <v>1.33</v>
+        <v>154.341</v>
       </c>
       <c r="B244" t="n">
-        <v>1.33</v>
+        <v>154.341</v>
       </c>
     </row>
     <row r="245">
@@ -2259,26 +2263,26 @@
     </row>
     <row r="246">
       <c r="A246" t="n">
-        <v>1.2</v>
+        <v>271.867</v>
       </c>
       <c r="B246" t="n">
-        <v>1.2</v>
+        <v>271.867</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="n">
-        <v>1.2</v>
+        <v>94.87</v>
       </c>
       <c r="B247" t="n">
-        <v>1.2</v>
+        <v>94.87</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="n">
-        <v>1.31</v>
+        <v>249.212</v>
       </c>
       <c r="B248" t="n">
-        <v>1.31</v>
+        <v>249.212</v>
       </c>
     </row>
     <row r="249">
@@ -2287,10 +2291,10 @@
     </row>
     <row r="250">
       <c r="A250" t="n">
-        <v>1.31</v>
+        <v>312.931</v>
       </c>
       <c r="B250" t="n">
-        <v>1.31</v>
+        <v>312.931</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add fifth workable version
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C84"/>
+  <dimension ref="A1:B84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,17 +436,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Скважины</t>
+          <t>Скважина+test_data_konkurs (1).xlsx ; УКПГ1АС</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Газ</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Добыча</t>
+          <t>Газ+test_data_konkurs (1).xlsx ; УКПГ1АС</t>
         </is>
       </c>
     </row>
@@ -457,14 +452,10 @@
       <c r="B2" t="n">
         <v>2096.235</v>
       </c>
-      <c r="C2" t="n">
-        <v>2096.235</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -473,9 +464,6 @@
       <c r="B4" t="n">
         <v>1841.123</v>
       </c>
-      <c r="C4" t="n">
-        <v>1841.123</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -484,14 +472,10 @@
       <c r="B5" t="n">
         <v>4757.68</v>
       </c>
-      <c r="C5" t="n">
-        <v>4757.68</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
       <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -500,14 +484,10 @@
       <c r="B7" t="n">
         <v>3943.907</v>
       </c>
-      <c r="C7" t="n">
-        <v>3943.907</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
       <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -516,9 +496,6 @@
       <c r="B9" t="n">
         <v>1404.648</v>
       </c>
-      <c r="C9" t="n">
-        <v>1404.648</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -527,9 +504,6 @@
       <c r="B10" t="n">
         <v>1536.334</v>
       </c>
-      <c r="C10" t="n">
-        <v>1536.334</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -538,9 +512,6 @@
       <c r="B11" t="n">
         <v>1536.334</v>
       </c>
-      <c r="C11" t="n">
-        <v>1536.334</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -549,9 +520,6 @@
       <c r="B12" t="n">
         <v>1931.392</v>
       </c>
-      <c r="C12" t="n">
-        <v>1931.392</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -560,9 +528,6 @@
       <c r="B13" t="n">
         <v>3116.564</v>
       </c>
-      <c r="C13" t="n">
-        <v>3116.564</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -571,9 +536,6 @@
       <c r="B14" t="n">
         <v>1753.45</v>
       </c>
-      <c r="C14" t="n">
-        <v>1753.45</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -582,9 +544,6 @@
       <c r="B15" t="n">
         <v>1753.45</v>
       </c>
-      <c r="C15" t="n">
-        <v>1753.45</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -593,9 +552,6 @@
       <c r="B16" t="n">
         <v>223.016</v>
       </c>
-      <c r="C16" t="n">
-        <v>223.016</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -604,9 +560,6 @@
       <c r="B17" t="n">
         <v>1536.334</v>
       </c>
-      <c r="C17" t="n">
-        <v>1536.334</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -615,9 +568,6 @@
       <c r="B18" t="n">
         <v>4082.26</v>
       </c>
-      <c r="C18" t="n">
-        <v>4082.26</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -626,9 +576,6 @@
       <c r="B19" t="n">
         <v>6891.557</v>
       </c>
-      <c r="C19" t="n">
-        <v>6891.557</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -637,14 +584,10 @@
       <c r="B20" t="n">
         <v>3981.961</v>
       </c>
-      <c r="C20" t="n">
-        <v>3981.961</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr"/>
       <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -653,14 +596,10 @@
       <c r="B22" t="n">
         <v>2123.964</v>
       </c>
-      <c r="C22" t="n">
-        <v>2123.964</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr"/>
       <c r="B23" t="inlineStr"/>
-      <c r="C23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -669,9 +608,6 @@
       <c r="B24" t="n">
         <v>2019.182</v>
       </c>
-      <c r="C24" t="n">
-        <v>2019.182</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -680,9 +616,6 @@
       <c r="B25" t="n">
         <v>1448.544</v>
       </c>
-      <c r="C25" t="n">
-        <v>1448.544</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -691,9 +624,6 @@
       <c r="B26" t="n">
         <v>1272.963</v>
       </c>
-      <c r="C26" t="n">
-        <v>1272.963</v>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -702,9 +632,6 @@
       <c r="B27" t="n">
         <v>3818.888</v>
       </c>
-      <c r="C27" t="n">
-        <v>3818.888</v>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -713,9 +640,6 @@
       <c r="B28" t="n">
         <v>5267.431</v>
       </c>
-      <c r="C28" t="n">
-        <v>5267.431</v>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -724,9 +648,6 @@
       <c r="B29" t="n">
         <v>4652.898</v>
       </c>
-      <c r="C29" t="n">
-        <v>4652.898</v>
-      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -735,9 +656,6 @@
       <c r="B30" t="n">
         <v>2414.24</v>
       </c>
-      <c r="C30" t="n">
-        <v>2414.24</v>
-      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -746,9 +664,6 @@
       <c r="B31" t="n">
         <v>2454.83</v>
       </c>
-      <c r="C31" t="n">
-        <v>2454.83</v>
-      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -757,19 +672,14 @@
       <c r="B32" t="n">
         <v>4478.025</v>
       </c>
-      <c r="C32" t="n">
-        <v>4478.025</v>
-      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr"/>
       <c r="B33" t="inlineStr"/>
-      <c r="C33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr"/>
       <c r="B34" t="inlineStr"/>
-      <c r="C34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -778,9 +688,6 @@
       <c r="B35" t="n">
         <v>5530.803</v>
       </c>
-      <c r="C35" t="n">
-        <v>5530.803</v>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -789,9 +696,6 @@
       <c r="B36" t="n">
         <v>1097.381</v>
       </c>
-      <c r="C36" t="n">
-        <v>1097.381</v>
-      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -800,14 +704,10 @@
       <c r="B37" t="n">
         <v>1974.343</v>
       </c>
-      <c r="C37" t="n">
-        <v>1974.343</v>
-      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr"/>
       <c r="B38" t="inlineStr"/>
-      <c r="C38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -816,9 +716,6 @@
       <c r="B39" t="n">
         <v>4652.898</v>
       </c>
-      <c r="C39" t="n">
-        <v>4652.898</v>
-      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -827,9 +724,6 @@
       <c r="B40" t="n">
         <v>5443.013</v>
       </c>
-      <c r="C40" t="n">
-        <v>5443.013</v>
-      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -838,14 +732,10 @@
       <c r="B41" t="n">
         <v>2747.289</v>
       </c>
-      <c r="C41" t="n">
-        <v>2747.289</v>
-      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr"/>
       <c r="B42" t="inlineStr"/>
-      <c r="C42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -854,9 +744,6 @@
       <c r="B43" t="n">
         <v>2739.914</v>
       </c>
-      <c r="C43" t="n">
-        <v>2739.914</v>
-      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -865,14 +752,10 @@
       <c r="B44" t="n">
         <v>5355.222</v>
       </c>
-      <c r="C44" t="n">
-        <v>5355.222</v>
-      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr"/>
       <c r="B45" t="inlineStr"/>
-      <c r="C45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -881,9 +764,6 @@
       <c r="B46" t="n">
         <v>5750.279</v>
       </c>
-      <c r="C46" t="n">
-        <v>5750.279</v>
-      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -892,9 +772,6 @@
       <c r="B47" t="n">
         <v>4565.107</v>
       </c>
-      <c r="C47" t="n">
-        <v>4565.107</v>
-      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -903,9 +780,6 @@
       <c r="B48" t="n">
         <v>4433.422</v>
       </c>
-      <c r="C48" t="n">
-        <v>4433.422</v>
-      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -914,9 +788,6 @@
       <c r="B49" t="n">
         <v>3511.621</v>
       </c>
-      <c r="C49" t="n">
-        <v>3511.621</v>
-      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -925,9 +796,6 @@
       <c r="B50" t="n">
         <v>3028.773</v>
       </c>
-      <c r="C50" t="n">
-        <v>3028.773</v>
-      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -936,9 +804,6 @@
       <c r="B51" t="n">
         <v>4170.05</v>
       </c>
-      <c r="C51" t="n">
-        <v>4170.05</v>
-      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -947,9 +812,6 @@
       <c r="B52" t="n">
         <v>2545.925</v>
       </c>
-      <c r="C52" t="n">
-        <v>2545.925</v>
-      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -958,9 +820,6 @@
       <c r="B53" t="n">
         <v>5047.955</v>
       </c>
-      <c r="C53" t="n">
-        <v>5047.955</v>
-      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -969,9 +828,6 @@
       <c r="B54" t="n">
         <v>6496.499</v>
       </c>
-      <c r="C54" t="n">
-        <v>6496.499</v>
-      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -980,9 +836,6 @@
       <c r="B55" t="n">
         <v>5925.86</v>
       </c>
-      <c r="C55" t="n">
-        <v>5925.86</v>
-      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -991,9 +844,6 @@
       <c r="B56" t="n">
         <v>8603.472</v>
       </c>
-      <c r="C56" t="n">
-        <v>8603.472</v>
-      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -1002,9 +852,6 @@
       <c r="B57" t="n">
         <v>3331.556</v>
       </c>
-      <c r="C57" t="n">
-        <v>3331.556</v>
-      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -1013,9 +860,6 @@
       <c r="B58" t="n">
         <v>7901.148</v>
       </c>
-      <c r="C58" t="n">
-        <v>7901.148</v>
-      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -1024,9 +868,6 @@
       <c r="B59" t="n">
         <v>6189.232</v>
       </c>
-      <c r="C59" t="n">
-        <v>6189.232</v>
-      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -1035,9 +876,6 @@
       <c r="B60" t="n">
         <v>5486.908</v>
       </c>
-      <c r="C60" t="n">
-        <v>5486.908</v>
-      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -1046,9 +884,6 @@
       <c r="B61" t="n">
         <v>2106.973</v>
       </c>
-      <c r="C61" t="n">
-        <v>2106.973</v>
-      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -1057,9 +892,6 @@
       <c r="B62" t="n">
         <v>4352.711</v>
       </c>
-      <c r="C62" t="n">
-        <v>4352.711</v>
-      </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -1068,9 +900,6 @@
       <c r="B63" t="n">
         <v>4521.212</v>
       </c>
-      <c r="C63" t="n">
-        <v>4521.212</v>
-      </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -1079,9 +908,6 @@
       <c r="B64" t="n">
         <v>4257.84</v>
       </c>
-      <c r="C64" t="n">
-        <v>4257.84</v>
-      </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -1090,9 +916,6 @@
       <c r="B65" t="n">
         <v>8735.156999999999</v>
       </c>
-      <c r="C65" t="n">
-        <v>8735.156999999999</v>
-      </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -1101,9 +924,6 @@
       <c r="B66" t="n">
         <v>8735.156999999999</v>
       </c>
-      <c r="C66" t="n">
-        <v>8735.156999999999</v>
-      </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -1112,9 +932,6 @@
       <c r="B67" t="n">
         <v>6891.557</v>
       </c>
-      <c r="C67" t="n">
-        <v>6891.557</v>
-      </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -1123,9 +940,6 @@
       <c r="B68" t="n">
         <v>5618.594</v>
       </c>
-      <c r="C68" t="n">
-        <v>5618.594</v>
-      </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -1134,9 +948,6 @@
       <c r="B69" t="n">
         <v>3336.04</v>
       </c>
-      <c r="C69" t="n">
-        <v>3336.04</v>
-      </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -1145,9 +956,6 @@
       <c r="B70" t="n">
         <v>5223.536</v>
       </c>
-      <c r="C70" t="n">
-        <v>5223.536</v>
-      </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -1156,9 +964,6 @@
       <c r="B71" t="n">
         <v>5530.803</v>
       </c>
-      <c r="C71" t="n">
-        <v>5530.803</v>
-      </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
@@ -1167,9 +972,6 @@
       <c r="B72" t="n">
         <v>9305.796</v>
       </c>
-      <c r="C72" t="n">
-        <v>9305.796</v>
-      </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
@@ -1178,9 +980,6 @@
       <c r="B73" t="n">
         <v>5706.384</v>
       </c>
-      <c r="C73" t="n">
-        <v>5706.384</v>
-      </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
@@ -1189,9 +988,6 @@
       <c r="B74" t="n">
         <v>3643.306</v>
       </c>
-      <c r="C74" t="n">
-        <v>3643.306</v>
-      </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -1200,9 +996,6 @@
       <c r="B75" t="n">
         <v>4740.689</v>
       </c>
-      <c r="C75" t="n">
-        <v>4740.689</v>
-      </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -1211,9 +1004,6 @@
       <c r="B76" t="n">
         <v>6759.87</v>
       </c>
-      <c r="C76" t="n">
-        <v>6759.87</v>
-      </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -1222,9 +1012,6 @@
       <c r="B77" t="n">
         <v>4696.793</v>
       </c>
-      <c r="C77" t="n">
-        <v>4696.793</v>
-      </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -1233,14 +1020,10 @@
       <c r="B78" t="n">
         <v>4475.901</v>
       </c>
-      <c r="C78" t="n">
-        <v>4475.901</v>
-      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr"/>
       <c r="B79" t="inlineStr"/>
-      <c r="C79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="n">
@@ -1249,9 +1032,6 @@
       <c r="B80" t="n">
         <v>8427.889999999999</v>
       </c>
-      <c r="C80" t="n">
-        <v>8427.889999999999</v>
-      </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -1260,9 +1040,6 @@
       <c r="B81" t="n">
         <v>2940.982</v>
       </c>
-      <c r="C81" t="n">
-        <v>2940.982</v>
-      </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
@@ -1271,23 +1048,16 @@
       <c r="B82" t="n">
         <v>6521.043</v>
       </c>
-      <c r="C82" t="n">
-        <v>6521.043</v>
-      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr"/>
       <c r="B83" t="inlineStr"/>
-      <c r="C83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="n">
         <v>1901</v>
       </c>
       <c r="B84" t="n">
-        <v>9700.852000000001</v>
-      </c>
-      <c r="C84" t="n">
         <v>9700.852000000001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add sixth workable version
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B84"/>
+  <dimension ref="A1:F84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +441,27 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Скважина+test_data_konkurs_.xlsx ; УКПГ1АС (2)</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Скважина+test_data_konkurs_.xlsx ; УКПГ1АС</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Газ+test_data_konkurs (1).xlsx ; УКПГ1АС</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Газ+test_data_konkurs_.xlsx ; УКПГ1АС (2)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Газ+test_data_konkurs_.xlsx ; УКПГ1АС</t>
         </is>
       </c>
     </row>
@@ -450,18 +470,46 @@
         <v>1591</v>
       </c>
       <c r="B2" t="n">
+        <v>1254.7</v>
+      </c>
+      <c r="C2" t="n">
+        <v>77.879</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2096.235</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2096.235</v>
+      </c>
+      <c r="F2" t="n">
         <v>2096.235</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
         <v>1620</v>
       </c>
       <c r="B4" t="n">
+        <v>1166.85</v>
+      </c>
+      <c r="C4" t="n">
+        <v>59.471</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1841.123</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1841.123</v>
+      </c>
+      <c r="F4" t="n">
         <v>1841.123</v>
       </c>
     </row>
@@ -470,30 +518,74 @@
         <v>1630</v>
       </c>
       <c r="B5" t="n">
+        <v>1193.92</v>
+      </c>
+      <c r="C5" t="n">
+        <v>158.589</v>
+      </c>
+      <c r="D5" t="n">
+        <v>4757.68</v>
+      </c>
+      <c r="E5" t="n">
+        <v>4757.68</v>
+      </c>
+      <c r="F5" t="n">
         <v>4757.68</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
       <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
         <v>1631</v>
       </c>
       <c r="B7" t="n">
+        <v>1218.9</v>
+      </c>
+      <c r="C7" t="n">
+        <v>145.846</v>
+      </c>
+      <c r="D7" t="n">
+        <v>3943.907</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3943.907</v>
+      </c>
+      <c r="F7" t="n">
         <v>3943.907</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
       <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
         <v>1640</v>
       </c>
       <c r="B9" t="n">
+        <v>1160</v>
+      </c>
+      <c r="C9" t="n">
+        <v>45.311</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1404.648</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1404.648</v>
+      </c>
+      <c r="F9" t="n">
         <v>1404.648</v>
       </c>
     </row>
@@ -502,6 +594,18 @@
         <v>1641</v>
       </c>
       <c r="B10" t="n">
+        <v>1174.4</v>
+      </c>
+      <c r="C10" t="n">
+        <v>49.559</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1536.334</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1536.334</v>
+      </c>
+      <c r="F10" t="n">
         <v>1536.334</v>
       </c>
     </row>
@@ -510,6 +614,18 @@
         <v>1642</v>
       </c>
       <c r="B11" t="n">
+        <v>1185.4</v>
+      </c>
+      <c r="C11" t="n">
+        <v>49.559</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1536.334</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1536.334</v>
+      </c>
+      <c r="F11" t="n">
         <v>1536.334</v>
       </c>
     </row>
@@ -518,6 +634,18 @@
         <v>1650</v>
       </c>
       <c r="B12" t="n">
+        <v>1169.5</v>
+      </c>
+      <c r="C12" t="n">
+        <v>62.303</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1931.392</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1931.392</v>
+      </c>
+      <c r="F12" t="n">
         <v>1931.392</v>
       </c>
     </row>
@@ -526,6 +654,18 @@
         <v>1651</v>
       </c>
       <c r="B13" t="n">
+        <v>1185.77</v>
+      </c>
+      <c r="C13" t="n">
+        <v>100.534</v>
+      </c>
+      <c r="D13" t="n">
+        <v>3116.564</v>
+      </c>
+      <c r="E13" t="n">
+        <v>3116.564</v>
+      </c>
+      <c r="F13" t="n">
         <v>3116.564</v>
       </c>
     </row>
@@ -534,6 +674,18 @@
         <v>1660</v>
       </c>
       <c r="B14" t="n">
+        <v>1161.72</v>
+      </c>
+      <c r="C14" t="n">
+        <v>56.639</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1753.45</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1753.45</v>
+      </c>
+      <c r="F14" t="n">
         <v>1753.45</v>
       </c>
     </row>
@@ -542,6 +694,18 @@
         <v>1661</v>
       </c>
       <c r="B15" t="n">
+        <v>1159</v>
+      </c>
+      <c r="C15" t="n">
+        <v>56.639</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1753.45</v>
+      </c>
+      <c r="E15" t="n">
+        <v>1753.45</v>
+      </c>
+      <c r="F15" t="n">
         <v>1753.45</v>
       </c>
     </row>
@@ -550,6 +714,18 @@
         <v>1662</v>
       </c>
       <c r="B16" t="n">
+        <v>1175.5</v>
+      </c>
+      <c r="C16" t="n">
+        <v>84.958</v>
+      </c>
+      <c r="D16" t="n">
+        <v>223.016</v>
+      </c>
+      <c r="E16" t="n">
+        <v>223.016</v>
+      </c>
+      <c r="F16" t="n">
         <v>223.016</v>
       </c>
     </row>
@@ -558,6 +734,18 @@
         <v>1670</v>
       </c>
       <c r="B17" t="n">
+        <v>1173.5</v>
+      </c>
+      <c r="C17" t="n">
+        <v>49.559</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1536.334</v>
+      </c>
+      <c r="E17" t="n">
+        <v>1536.334</v>
+      </c>
+      <c r="F17" t="n">
         <v>1536.334</v>
       </c>
     </row>
@@ -566,6 +754,18 @@
         <v>1671</v>
       </c>
       <c r="B18" t="n">
+        <v>1213.2</v>
+      </c>
+      <c r="C18" t="n">
+        <v>131.686</v>
+      </c>
+      <c r="D18" t="n">
+        <v>4082.26</v>
+      </c>
+      <c r="E18" t="n">
+        <v>4082.26</v>
+      </c>
+      <c r="F18" t="n">
         <v>4082.26</v>
       </c>
     </row>
@@ -574,6 +774,18 @@
         <v>1680</v>
       </c>
       <c r="B19" t="n">
+        <v>1132.3</v>
+      </c>
+      <c r="C19" t="n">
+        <v>222.308</v>
+      </c>
+      <c r="D19" t="n">
+        <v>6891.557</v>
+      </c>
+      <c r="E19" t="n">
+        <v>6891.557</v>
+      </c>
+      <c r="F19" t="n">
         <v>6891.557</v>
       </c>
     </row>
@@ -582,30 +794,76 @@
         <v>1681</v>
       </c>
       <c r="B20" t="n">
+        <v>1218.2</v>
+      </c>
+      <c r="C20" t="n">
+        <v>133.102</v>
+      </c>
+      <c r="D20" t="n">
+        <v>3981.961</v>
+      </c>
+      <c r="E20" t="n">
+        <v>3981.961</v>
+      </c>
+      <c r="F20" t="n">
         <v>3981.961</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr"/>
       <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
         <v>1682</v>
       </c>
       <c r="B22" t="n">
+        <v>1018.36</v>
+      </c>
+      <c r="C22" t="n">
+        <v>70.79900000000001</v>
+      </c>
+      <c r="D22" t="n">
+        <v>2123.964</v>
+      </c>
+      <c r="E22" t="n">
+        <v>2123.964</v>
+      </c>
+      <c r="F22" t="n">
         <v>2123.964</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr"/>
-      <c r="B23" t="inlineStr"/>
+      <c r="B23" t="n">
+        <v>1198.9</v>
+      </c>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
         <v>1690</v>
       </c>
       <c r="B24" t="n">
+        <v>1159.77</v>
+      </c>
+      <c r="C24" t="n">
+        <v>65.13500000000001</v>
+      </c>
+      <c r="D24" t="n">
+        <v>2019.182</v>
+      </c>
+      <c r="E24" t="n">
+        <v>2019.182</v>
+      </c>
+      <c r="F24" t="n">
         <v>2019.182</v>
       </c>
     </row>
@@ -614,6 +872,18 @@
         <v>1691</v>
       </c>
       <c r="B25" t="n">
+        <v>1191.2</v>
+      </c>
+      <c r="C25" t="n">
+        <v>46.727</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1448.544</v>
+      </c>
+      <c r="E25" t="n">
+        <v>1448.544</v>
+      </c>
+      <c r="F25" t="n">
         <v>1448.544</v>
       </c>
     </row>
@@ -622,6 +892,18 @@
         <v>1700</v>
       </c>
       <c r="B26" t="n">
+        <v>1180.3</v>
+      </c>
+      <c r="C26" t="n">
+        <v>41.063</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1272.963</v>
+      </c>
+      <c r="E26" t="n">
+        <v>1272.963</v>
+      </c>
+      <c r="F26" t="n">
         <v>1272.963</v>
       </c>
     </row>
@@ -630,6 +912,18 @@
         <v>1701</v>
       </c>
       <c r="B27" t="n">
+        <v>1214.4</v>
+      </c>
+      <c r="C27" t="n">
+        <v>123.19</v>
+      </c>
+      <c r="D27" t="n">
+        <v>3818.888</v>
+      </c>
+      <c r="E27" t="n">
+        <v>3818.888</v>
+      </c>
+      <c r="F27" t="n">
         <v>3818.888</v>
       </c>
     </row>
@@ -638,6 +932,18 @@
         <v>1702</v>
       </c>
       <c r="B28" t="n">
+        <v>1135.6</v>
+      </c>
+      <c r="C28" t="n">
+        <v>169.917</v>
+      </c>
+      <c r="D28" t="n">
+        <v>5267.431</v>
+      </c>
+      <c r="E28" t="n">
+        <v>5267.431</v>
+      </c>
+      <c r="F28" t="n">
         <v>5267.431</v>
       </c>
     </row>
@@ -646,6 +952,18 @@
         <v>1710</v>
       </c>
       <c r="B29" t="n">
+        <v>1152.3</v>
+      </c>
+      <c r="C29" t="n">
+        <v>150.093</v>
+      </c>
+      <c r="D29" t="n">
+        <v>4652.898</v>
+      </c>
+      <c r="E29" t="n">
+        <v>4652.898</v>
+      </c>
+      <c r="F29" t="n">
         <v>4652.898</v>
       </c>
     </row>
@@ -654,6 +972,18 @@
         <v>1711</v>
       </c>
       <c r="B30" t="n">
+        <v>1211.95</v>
+      </c>
+      <c r="C30" t="n">
+        <v>77.879</v>
+      </c>
+      <c r="D30" t="n">
+        <v>2414.24</v>
+      </c>
+      <c r="E30" t="n">
+        <v>2414.24</v>
+      </c>
+      <c r="F30" t="n">
         <v>2414.24</v>
       </c>
     </row>
@@ -662,6 +992,18 @@
         <v>1720</v>
       </c>
       <c r="B31" t="n">
+        <v>1201.8</v>
+      </c>
+      <c r="C31" t="n">
+        <v>79.295</v>
+      </c>
+      <c r="D31" t="n">
+        <v>2454.83</v>
+      </c>
+      <c r="E31" t="n">
+        <v>2454.83</v>
+      </c>
+      <c r="F31" t="n">
         <v>2454.83</v>
       </c>
     </row>
@@ -670,22 +1012,54 @@
         <v>1721</v>
       </c>
       <c r="B32" t="n">
+        <v>1163.1</v>
+      </c>
+      <c r="C32" t="n">
+        <v>155.757</v>
+      </c>
+      <c r="D32" t="n">
+        <v>4478.025</v>
+      </c>
+      <c r="E32" t="n">
+        <v>4478.025</v>
+      </c>
+      <c r="F32" t="n">
         <v>4478.025</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr"/>
       <c r="B33" t="inlineStr"/>
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr"/>
       <c r="B34" t="inlineStr"/>
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="inlineStr"/>
+      <c r="F34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
         <v>1730</v>
       </c>
       <c r="B35" t="n">
+        <v>1172.9</v>
+      </c>
+      <c r="C35" t="n">
+        <v>178.413</v>
+      </c>
+      <c r="D35" t="n">
+        <v>5530.803</v>
+      </c>
+      <c r="E35" t="n">
+        <v>5530.803</v>
+      </c>
+      <c r="F35" t="n">
         <v>5530.803</v>
       </c>
     </row>
@@ -694,6 +1068,18 @@
         <v>1731</v>
       </c>
       <c r="B36" t="n">
+        <v>1175.4</v>
+      </c>
+      <c r="C36" t="n">
+        <v>35.399</v>
+      </c>
+      <c r="D36" t="n">
+        <v>1097.381</v>
+      </c>
+      <c r="E36" t="n">
+        <v>1097.381</v>
+      </c>
+      <c r="F36" t="n">
         <v>1097.381</v>
       </c>
     </row>
@@ -702,18 +1088,46 @@
         <v>1740</v>
       </c>
       <c r="B37" t="n">
+        <v>1175.7</v>
+      </c>
+      <c r="C37" t="n">
+        <v>66.551</v>
+      </c>
+      <c r="D37" t="n">
+        <v>1974.343</v>
+      </c>
+      <c r="E37" t="n">
+        <v>1974.343</v>
+      </c>
+      <c r="F37" t="n">
         <v>1974.343</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr"/>
       <c r="B38" t="inlineStr"/>
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="inlineStr"/>
+      <c r="E38" t="inlineStr"/>
+      <c r="F38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="n">
         <v>1741</v>
       </c>
       <c r="B39" t="n">
+        <v>1183.2</v>
+      </c>
+      <c r="C39" t="n">
+        <v>150.093</v>
+      </c>
+      <c r="D39" t="n">
+        <v>4652.898</v>
+      </c>
+      <c r="E39" t="n">
+        <v>4652.898</v>
+      </c>
+      <c r="F39" t="n">
         <v>4652.898</v>
       </c>
     </row>
@@ -722,6 +1136,18 @@
         <v>1750</v>
       </c>
       <c r="B40" t="n">
+        <v>1184.8</v>
+      </c>
+      <c r="C40" t="n">
+        <v>175.581</v>
+      </c>
+      <c r="D40" t="n">
+        <v>5443.013</v>
+      </c>
+      <c r="E40" t="n">
+        <v>5443.013</v>
+      </c>
+      <c r="F40" t="n">
         <v>5443.013</v>
       </c>
     </row>
@@ -730,18 +1156,46 @@
         <v>1751</v>
       </c>
       <c r="B41" t="n">
+        <v>1173.4</v>
+      </c>
+      <c r="C41" t="n">
+        <v>94.87</v>
+      </c>
+      <c r="D41" t="n">
+        <v>2747.289</v>
+      </c>
+      <c r="E41" t="n">
+        <v>2747.289</v>
+      </c>
+      <c r="F41" t="n">
         <v>2747.289</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr"/>
       <c r="B42" t="inlineStr"/>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="inlineStr"/>
+      <c r="F42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="n">
         <v>1752</v>
       </c>
       <c r="B43" t="n">
+        <v>1184.57</v>
+      </c>
+      <c r="C43" t="n">
+        <v>101.95</v>
+      </c>
+      <c r="D43" t="n">
+        <v>2739.914</v>
+      </c>
+      <c r="E43" t="n">
+        <v>2739.914</v>
+      </c>
+      <c r="F43" t="n">
         <v>2739.914</v>
       </c>
     </row>
@@ -750,18 +1204,48 @@
         <v>1770</v>
       </c>
       <c r="B44" t="n">
+        <v>941.5</v>
+      </c>
+      <c r="C44" t="n">
+        <v>172.749</v>
+      </c>
+      <c r="D44" t="n">
+        <v>5355.222</v>
+      </c>
+      <c r="E44" t="n">
+        <v>5355.222</v>
+      </c>
+      <c r="F44" t="n">
         <v>5355.222</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr"/>
-      <c r="B45" t="inlineStr"/>
+      <c r="B45" t="n">
+        <v>1155.9</v>
+      </c>
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="inlineStr"/>
+      <c r="E45" t="inlineStr"/>
+      <c r="F45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
         <v>1771</v>
       </c>
       <c r="B46" t="n">
+        <v>1159.7</v>
+      </c>
+      <c r="C46" t="n">
+        <v>185.493</v>
+      </c>
+      <c r="D46" t="n">
+        <v>5750.279</v>
+      </c>
+      <c r="E46" t="n">
+        <v>5750.279</v>
+      </c>
+      <c r="F46" t="n">
         <v>5750.279</v>
       </c>
     </row>
@@ -770,6 +1254,18 @@
         <v>1780</v>
       </c>
       <c r="B47" t="n">
+        <v>1184.7</v>
+      </c>
+      <c r="C47" t="n">
+        <v>147.262</v>
+      </c>
+      <c r="D47" t="n">
+        <v>4565.107</v>
+      </c>
+      <c r="E47" t="n">
+        <v>4565.107</v>
+      </c>
+      <c r="F47" t="n">
         <v>4565.107</v>
       </c>
     </row>
@@ -778,6 +1274,18 @@
         <v>1781</v>
       </c>
       <c r="B48" t="n">
+        <v>1188.9</v>
+      </c>
+      <c r="C48" t="n">
+        <v>143.014</v>
+      </c>
+      <c r="D48" t="n">
+        <v>4433.422</v>
+      </c>
+      <c r="E48" t="n">
+        <v>4433.422</v>
+      </c>
+      <c r="F48" t="n">
         <v>4433.422</v>
       </c>
     </row>
@@ -786,6 +1294,18 @@
         <v>1782</v>
       </c>
       <c r="B49" t="n">
+        <v>1181.2</v>
+      </c>
+      <c r="C49" t="n">
+        <v>113.278</v>
+      </c>
+      <c r="D49" t="n">
+        <v>3511.621</v>
+      </c>
+      <c r="E49" t="n">
+        <v>3511.621</v>
+      </c>
+      <c r="F49" t="n">
         <v>3511.621</v>
       </c>
     </row>
@@ -794,6 +1314,18 @@
         <v>1790</v>
       </c>
       <c r="B50" t="n">
+        <v>1143.8</v>
+      </c>
+      <c r="C50" t="n">
+        <v>97.702</v>
+      </c>
+      <c r="D50" t="n">
+        <v>3028.773</v>
+      </c>
+      <c r="E50" t="n">
+        <v>3028.773</v>
+      </c>
+      <c r="F50" t="n">
         <v>3028.773</v>
       </c>
     </row>
@@ -802,6 +1334,18 @@
         <v>1791</v>
       </c>
       <c r="B51" t="n">
+        <v>1224.3</v>
+      </c>
+      <c r="C51" t="n">
+        <v>134.518</v>
+      </c>
+      <c r="D51" t="n">
+        <v>4170.05</v>
+      </c>
+      <c r="E51" t="n">
+        <v>4170.05</v>
+      </c>
+      <c r="F51" t="n">
         <v>4170.05</v>
       </c>
     </row>
@@ -810,6 +1354,18 @@
         <v>1792</v>
       </c>
       <c r="B52" t="n">
+        <v>1189.9</v>
+      </c>
+      <c r="C52" t="n">
+        <v>82.127</v>
+      </c>
+      <c r="D52" t="n">
+        <v>2545.925</v>
+      </c>
+      <c r="E52" t="n">
+        <v>2545.925</v>
+      </c>
+      <c r="F52" t="n">
         <v>2545.925</v>
       </c>
     </row>
@@ -818,6 +1374,18 @@
         <v>1800</v>
       </c>
       <c r="B53" t="n">
+        <v>1203.4</v>
+      </c>
+      <c r="C53" t="n">
+        <v>162.837</v>
+      </c>
+      <c r="D53" t="n">
+        <v>5047.955</v>
+      </c>
+      <c r="E53" t="n">
+        <v>5047.955</v>
+      </c>
+      <c r="F53" t="n">
         <v>5047.955</v>
       </c>
     </row>
@@ -826,6 +1394,18 @@
         <v>1801</v>
       </c>
       <c r="B54" t="n">
+        <v>1153</v>
+      </c>
+      <c r="C54" t="n">
+        <v>209.564</v>
+      </c>
+      <c r="D54" t="n">
+        <v>6496.499</v>
+      </c>
+      <c r="E54" t="n">
+        <v>6496.499</v>
+      </c>
+      <c r="F54" t="n">
         <v>6496.499</v>
       </c>
     </row>
@@ -834,6 +1414,18 @@
         <v>1802</v>
       </c>
       <c r="B55" t="n">
+        <v>1178.8</v>
+      </c>
+      <c r="C55" t="n">
+        <v>191.157</v>
+      </c>
+      <c r="D55" t="n">
+        <v>5925.86</v>
+      </c>
+      <c r="E55" t="n">
+        <v>5925.86</v>
+      </c>
+      <c r="F55" t="n">
         <v>5925.86</v>
       </c>
     </row>
@@ -842,6 +1434,18 @@
         <v>1810</v>
       </c>
       <c r="B56" t="n">
+        <v>1183.8</v>
+      </c>
+      <c r="C56" t="n">
+        <v>277.531</v>
+      </c>
+      <c r="D56" t="n">
+        <v>8603.472</v>
+      </c>
+      <c r="E56" t="n">
+        <v>8603.472</v>
+      </c>
+      <c r="F56" t="n">
         <v>8603.472</v>
       </c>
     </row>
@@ -850,6 +1454,18 @@
         <v>1811</v>
       </c>
       <c r="B57" t="n">
+        <v>1214.7</v>
+      </c>
+      <c r="C57" t="n">
+        <v>107.614</v>
+      </c>
+      <c r="D57" t="n">
+        <v>3331.556</v>
+      </c>
+      <c r="E57" t="n">
+        <v>3331.556</v>
+      </c>
+      <c r="F57" t="n">
         <v>3331.556</v>
       </c>
     </row>
@@ -858,6 +1474,18 @@
         <v>1812</v>
       </c>
       <c r="B58" t="n">
+        <v>1154.2</v>
+      </c>
+      <c r="C58" t="n">
+        <v>254.876</v>
+      </c>
+      <c r="D58" t="n">
+        <v>7901.148</v>
+      </c>
+      <c r="E58" t="n">
+        <v>7901.148</v>
+      </c>
+      <c r="F58" t="n">
         <v>7901.148</v>
       </c>
     </row>
@@ -866,6 +1494,18 @@
         <v>1820</v>
       </c>
       <c r="B59" t="n">
+        <v>1201.8</v>
+      </c>
+      <c r="C59" t="n">
+        <v>199.653</v>
+      </c>
+      <c r="D59" t="n">
+        <v>6189.232</v>
+      </c>
+      <c r="E59" t="n">
+        <v>6189.232</v>
+      </c>
+      <c r="F59" t="n">
         <v>6189.232</v>
       </c>
     </row>
@@ -874,6 +1514,18 @@
         <v>1821</v>
       </c>
       <c r="B60" t="n">
+        <v>1164.7</v>
+      </c>
+      <c r="C60" t="n">
+        <v>176.997</v>
+      </c>
+      <c r="D60" t="n">
+        <v>5486.908</v>
+      </c>
+      <c r="E60" t="n">
+        <v>5486.908</v>
+      </c>
+      <c r="F60" t="n">
         <v>5486.908</v>
       </c>
     </row>
@@ -882,6 +1534,18 @@
         <v>1822</v>
       </c>
       <c r="B61" t="n">
+        <v>1202.19</v>
+      </c>
+      <c r="C61" t="n">
+        <v>67.967</v>
+      </c>
+      <c r="D61" t="n">
+        <v>2106.973</v>
+      </c>
+      <c r="E61" t="n">
+        <v>2106.973</v>
+      </c>
+      <c r="F61" t="n">
         <v>2106.973</v>
       </c>
     </row>
@@ -890,6 +1554,18 @@
         <v>1830</v>
       </c>
       <c r="B62" t="n">
+        <v>1181.3</v>
+      </c>
+      <c r="C62" t="n">
+        <v>150.093</v>
+      </c>
+      <c r="D62" t="n">
+        <v>4352.711</v>
+      </c>
+      <c r="E62" t="n">
+        <v>4352.711</v>
+      </c>
+      <c r="F62" t="n">
         <v>4352.711</v>
       </c>
     </row>
@@ -898,6 +1574,18 @@
         <v>1831</v>
       </c>
       <c r="B63" t="n">
+        <v>1166.2</v>
+      </c>
+      <c r="C63" t="n">
+        <v>145.846</v>
+      </c>
+      <c r="D63" t="n">
+        <v>4521.212</v>
+      </c>
+      <c r="E63" t="n">
+        <v>4521.212</v>
+      </c>
+      <c r="F63" t="n">
         <v>4521.212</v>
       </c>
     </row>
@@ -906,6 +1594,18 @@
         <v>1832</v>
       </c>
       <c r="B64" t="n">
+        <v>1175.27</v>
+      </c>
+      <c r="C64" t="n">
+        <v>137.35</v>
+      </c>
+      <c r="D64" t="n">
+        <v>4257.84</v>
+      </c>
+      <c r="E64" t="n">
+        <v>4257.84</v>
+      </c>
+      <c r="F64" t="n">
         <v>4257.84</v>
       </c>
     </row>
@@ -914,6 +1614,18 @@
         <v>1840</v>
       </c>
       <c r="B65" t="n">
+        <v>1210.3</v>
+      </c>
+      <c r="C65" t="n">
+        <v>281.779</v>
+      </c>
+      <c r="D65" t="n">
+        <v>8735.156999999999</v>
+      </c>
+      <c r="E65" t="n">
+        <v>8735.156999999999</v>
+      </c>
+      <c r="F65" t="n">
         <v>8735.156999999999</v>
       </c>
     </row>
@@ -922,6 +1634,18 @@
         <v>1841</v>
       </c>
       <c r="B66" t="n">
+        <v>1174.1</v>
+      </c>
+      <c r="C66" t="n">
+        <v>281.779</v>
+      </c>
+      <c r="D66" t="n">
+        <v>8735.156999999999</v>
+      </c>
+      <c r="E66" t="n">
+        <v>8735.156999999999</v>
+      </c>
+      <c r="F66" t="n">
         <v>8735.156999999999</v>
       </c>
     </row>
@@ -930,6 +1654,18 @@
         <v>1842</v>
       </c>
       <c r="B67" t="n">
+        <v>1222.7</v>
+      </c>
+      <c r="C67" t="n">
+        <v>222.308</v>
+      </c>
+      <c r="D67" t="n">
+        <v>6891.557</v>
+      </c>
+      <c r="E67" t="n">
+        <v>6891.557</v>
+      </c>
+      <c r="F67" t="n">
         <v>6891.557</v>
       </c>
     </row>
@@ -938,6 +1674,18 @@
         <v>1850</v>
       </c>
       <c r="B68" t="n">
+        <v>1160.4</v>
+      </c>
+      <c r="C68" t="n">
+        <v>181.245</v>
+      </c>
+      <c r="D68" t="n">
+        <v>5618.594</v>
+      </c>
+      <c r="E68" t="n">
+        <v>5618.594</v>
+      </c>
+      <c r="F68" t="n">
         <v>5618.594</v>
       </c>
     </row>
@@ -946,6 +1694,18 @@
         <v>1851</v>
       </c>
       <c r="B69" t="n">
+        <v>1146.8</v>
+      </c>
+      <c r="C69" t="n">
+        <v>107.614</v>
+      </c>
+      <c r="D69" t="n">
+        <v>3336.04</v>
+      </c>
+      <c r="E69" t="n">
+        <v>3336.04</v>
+      </c>
+      <c r="F69" t="n">
         <v>3336.04</v>
       </c>
     </row>
@@ -954,6 +1714,18 @@
         <v>1860</v>
       </c>
       <c r="B70" t="n">
+        <v>1189.9</v>
+      </c>
+      <c r="C70" t="n">
+        <v>168.501</v>
+      </c>
+      <c r="D70" t="n">
+        <v>5223.536</v>
+      </c>
+      <c r="E70" t="n">
+        <v>5223.536</v>
+      </c>
+      <c r="F70" t="n">
         <v>5223.536</v>
       </c>
     </row>
@@ -962,6 +1734,18 @@
         <v>1861</v>
       </c>
       <c r="B71" t="n">
+        <v>1209.5</v>
+      </c>
+      <c r="C71" t="n">
+        <v>178.413</v>
+      </c>
+      <c r="D71" t="n">
+        <v>5530.803</v>
+      </c>
+      <c r="E71" t="n">
+        <v>5530.803</v>
+      </c>
+      <c r="F71" t="n">
         <v>5530.803</v>
       </c>
     </row>
@@ -970,6 +1754,18 @@
         <v>1863</v>
       </c>
       <c r="B72" t="n">
+        <v>1184.5</v>
+      </c>
+      <c r="C72" t="n">
+        <v>300.187</v>
+      </c>
+      <c r="D72" t="n">
+        <v>9305.796</v>
+      </c>
+      <c r="E72" t="n">
+        <v>9305.796</v>
+      </c>
+      <c r="F72" t="n">
         <v>9305.796</v>
       </c>
     </row>
@@ -978,6 +1774,18 @@
         <v>1870</v>
       </c>
       <c r="B73" t="n">
+        <v>1182.5</v>
+      </c>
+      <c r="C73" t="n">
+        <v>184.077</v>
+      </c>
+      <c r="D73" t="n">
+        <v>5706.384</v>
+      </c>
+      <c r="E73" t="n">
+        <v>5706.384</v>
+      </c>
+      <c r="F73" t="n">
         <v>5706.384</v>
       </c>
     </row>
@@ -986,6 +1794,18 @@
         <v>1871</v>
       </c>
       <c r="B74" t="n">
+        <v>1189</v>
+      </c>
+      <c r="C74" t="n">
+        <v>117.526</v>
+      </c>
+      <c r="D74" t="n">
+        <v>3643.306</v>
+      </c>
+      <c r="E74" t="n">
+        <v>3643.306</v>
+      </c>
+      <c r="F74" t="n">
         <v>3643.306</v>
       </c>
     </row>
@@ -994,6 +1814,18 @@
         <v>1872</v>
       </c>
       <c r="B75" t="n">
+        <v>1216.5</v>
+      </c>
+      <c r="C75" t="n">
+        <v>152.925</v>
+      </c>
+      <c r="D75" t="n">
+        <v>4740.689</v>
+      </c>
+      <c r="E75" t="n">
+        <v>4740.689</v>
+      </c>
+      <c r="F75" t="n">
         <v>4740.689</v>
       </c>
     </row>
@@ -1002,6 +1834,18 @@
         <v>1880</v>
       </c>
       <c r="B76" t="n">
+        <v>1175</v>
+      </c>
+      <c r="C76" t="n">
+        <v>218.06</v>
+      </c>
+      <c r="D76" t="n">
+        <v>6759.87</v>
+      </c>
+      <c r="E76" t="n">
+        <v>6759.87</v>
+      </c>
+      <c r="F76" t="n">
         <v>6759.87</v>
       </c>
     </row>
@@ -1010,6 +1854,18 @@
         <v>1881</v>
       </c>
       <c r="B77" t="n">
+        <v>1141.9</v>
+      </c>
+      <c r="C77" t="n">
+        <v>151.509</v>
+      </c>
+      <c r="D77" t="n">
+        <v>4696.793</v>
+      </c>
+      <c r="E77" t="n">
+        <v>4696.793</v>
+      </c>
+      <c r="F77" t="n">
         <v>4696.793</v>
       </c>
     </row>
@@ -1018,18 +1874,46 @@
         <v>1882</v>
       </c>
       <c r="B78" t="n">
+        <v>1228</v>
+      </c>
+      <c r="C78" t="n">
+        <v>154.341</v>
+      </c>
+      <c r="D78" t="n">
+        <v>4475.901</v>
+      </c>
+      <c r="E78" t="n">
+        <v>4475.901</v>
+      </c>
+      <c r="F78" t="n">
         <v>4475.901</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr"/>
       <c r="B79" t="inlineStr"/>
+      <c r="C79" t="inlineStr"/>
+      <c r="D79" t="inlineStr"/>
+      <c r="E79" t="inlineStr"/>
+      <c r="F79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="n">
         <v>1890</v>
       </c>
       <c r="B80" t="n">
+        <v>1154.6</v>
+      </c>
+      <c r="C80" t="n">
+        <v>271.867</v>
+      </c>
+      <c r="D80" t="n">
+        <v>8427.889999999999</v>
+      </c>
+      <c r="E80" t="n">
+        <v>8427.889999999999</v>
+      </c>
+      <c r="F80" t="n">
         <v>8427.889999999999</v>
       </c>
     </row>
@@ -1038,6 +1922,18 @@
         <v>1891</v>
       </c>
       <c r="B81" t="n">
+        <v>1172.04</v>
+      </c>
+      <c r="C81" t="n">
+        <v>94.87</v>
+      </c>
+      <c r="D81" t="n">
+        <v>2940.982</v>
+      </c>
+      <c r="E81" t="n">
+        <v>2940.982</v>
+      </c>
+      <c r="F81" t="n">
         <v>2940.982</v>
       </c>
     </row>
@@ -1046,18 +1942,46 @@
         <v>1900</v>
       </c>
       <c r="B82" t="n">
+        <v>1203.9</v>
+      </c>
+      <c r="C82" t="n">
+        <v>249.212</v>
+      </c>
+      <c r="D82" t="n">
+        <v>6521.043</v>
+      </c>
+      <c r="E82" t="n">
+        <v>6521.043</v>
+      </c>
+      <c r="F82" t="n">
         <v>6521.043</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr"/>
       <c r="B83" t="inlineStr"/>
+      <c r="C83" t="inlineStr"/>
+      <c r="D83" t="inlineStr"/>
+      <c r="E83" t="inlineStr"/>
+      <c r="F83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="n">
         <v>1901</v>
       </c>
       <c r="B84" t="n">
+        <v>1160.7</v>
+      </c>
+      <c r="C84" t="n">
+        <v>312.931</v>
+      </c>
+      <c r="D84" t="n">
+        <v>9700.852000000001</v>
+      </c>
+      <c r="E84" t="n">
+        <v>9700.852000000001</v>
+      </c>
+      <c r="F84" t="n">
         <v>9700.852000000001</v>
       </c>
     </row>

</xml_diff>